<commit_message>
Apply constraints and attributes to all relevant regions
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_RES99.xlsx
+++ b/SuppXLS/Scen_ELC_RES99.xlsx
@@ -1,20 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\I3p0_ELC_12TS_1REG_2020.11.18\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09275155-0FE9-4815-97A8-D3D52AC9D90B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4EFB22-0091-4111-B3CA-29C21A6F0868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="Regions" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
+    <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
+    <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,8 +52,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="97">
   <si>
     <t>UC_N</t>
   </si>
@@ -88,9 +132,6 @@
   </si>
   <si>
     <t>RNW Level</t>
-  </si>
-  <si>
-    <t>~UC_Sets: R_E: IE</t>
   </si>
   <si>
     <t>~UC_T</t>
@@ -158,13 +199,211 @@
   <si>
     <t>P*HFO*</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>Single-region</t>
+  </si>
+  <si>
+    <t>Multi-region</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>County name</t>
+  </si>
+  <si>
+    <t>IE-CW</t>
+  </si>
+  <si>
+    <t>Carlow</t>
+  </si>
+  <si>
+    <t>IE-CN</t>
+  </si>
+  <si>
+    <t>Cavan</t>
+  </si>
+  <si>
+    <t>IE-CE</t>
+  </si>
+  <si>
+    <t>Clare</t>
+  </si>
+  <si>
+    <t>IE-CO</t>
+  </si>
+  <si>
+    <t>Cork</t>
+  </si>
+  <si>
+    <t>IE-DL</t>
+  </si>
+  <si>
+    <t>Donegal</t>
+  </si>
+  <si>
+    <t>IE-D</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>IE-G</t>
+  </si>
+  <si>
+    <t>Galway</t>
+  </si>
+  <si>
+    <t>IE-KY</t>
+  </si>
+  <si>
+    <t>Kerry</t>
+  </si>
+  <si>
+    <t>IE-KE</t>
+  </si>
+  <si>
+    <t>Kildare</t>
+  </si>
+  <si>
+    <t>IE-KK</t>
+  </si>
+  <si>
+    <t>Kilkenny</t>
+  </si>
+  <si>
+    <t>IE-LS</t>
+  </si>
+  <si>
+    <t>Laois</t>
+  </si>
+  <si>
+    <t>IE-LM</t>
+  </si>
+  <si>
+    <t>Leitrim</t>
+  </si>
+  <si>
+    <t>IE-LK</t>
+  </si>
+  <si>
+    <t>Limerick</t>
+  </si>
+  <si>
+    <t>IE-LD</t>
+  </si>
+  <si>
+    <t>Longford</t>
+  </si>
+  <si>
+    <t>IE-LH</t>
+  </si>
+  <si>
+    <t>Louth</t>
+  </si>
+  <si>
+    <t>IE-MO</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>IE-MH</t>
+  </si>
+  <si>
+    <t>Meath</t>
+  </si>
+  <si>
+    <t>IE-MN</t>
+  </si>
+  <si>
+    <t>Monaghan</t>
+  </si>
+  <si>
+    <t>IE-OY</t>
+  </si>
+  <si>
+    <t>Offaly</t>
+  </si>
+  <si>
+    <t>IE-RN</t>
+  </si>
+  <si>
+    <t>Roscommon</t>
+  </si>
+  <si>
+    <t>IE-SO</t>
+  </si>
+  <si>
+    <t>Sligo</t>
+  </si>
+  <si>
+    <t>IE-TA</t>
+  </si>
+  <si>
+    <t>Tipperary</t>
+  </si>
+  <si>
+    <t>IE-WD</t>
+  </si>
+  <si>
+    <t>Waterford</t>
+  </si>
+  <si>
+    <t>IE-WH</t>
+  </si>
+  <si>
+    <t>Westmeath</t>
+  </si>
+  <si>
+    <t>IE-WX</t>
+  </si>
+  <si>
+    <t>Wexford</t>
+  </si>
+  <si>
+    <t>IE-WW</t>
+  </si>
+  <si>
+    <t>Wicklow</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://en.wikipedia.org/wiki/ISO_3166-2:IE</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,16 +422,45 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -200,16 +468,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{34A05EA6-9999-4593-9DE7-38F37B7299EA}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -222,6 +563,90 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="39" fmlaLink="$A$4" fmlaRange="$A$5:$A$7" noThreeD="1" sel="1" val="0"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Drop Down 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D20E4213-9FEA-4A16-8861-FF938A32BC81}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Regions"/>
+      <sheetName val="UC_CCS"/>
+      <sheetName val="FLO_EMIS"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -544,24 +969,789 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A84AB881-5881-43E0-8698-29D47DB36E46}">
+  <dimension ref="A3:AD37"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="10.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="2.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="5.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="5.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="7.875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:30" ht="15">
+      <c r="C3" s="3" t="str" cm="1">
+        <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
+        <v>IE</v>
+      </c>
+      <c r="D3" s="3" t="str" cm="1">
+        <f t="array" ref="D3">INDEX(D5:D7,$A$4)</f>
+        <v>National</v>
+      </c>
+      <c r="E3" s="3" t="str" cm="1">
+        <f t="array" ref="E3">INDEX(E5:E7,$A$4)</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="F3" s="3" t="str" cm="1">
+        <f t="array" ref="F3">INDEX(F5:F7,$A$4)</f>
+        <v>IE-D</v>
+      </c>
+      <c r="G3" s="3" t="str" cm="1">
+        <f t="array" ref="G3">INDEX(G5:G7,$A$4)</f>
+        <v>IE-KE</v>
+      </c>
+      <c r="H3" s="3" t="str" cm="1">
+        <f t="array" ref="H3">INDEX(H5:H7,$A$4)</f>
+        <v>IE-KK</v>
+      </c>
+      <c r="I3" s="3" t="str" cm="1">
+        <f t="array" ref="I3">INDEX(I5:I7,$A$4)</f>
+        <v>IE-LS</v>
+      </c>
+      <c r="J3" s="3" t="str" cm="1">
+        <f t="array" ref="J3">INDEX(J5:J7,$A$4)</f>
+        <v>IE-LD</v>
+      </c>
+      <c r="K3" s="3" t="str" cm="1">
+        <f t="array" ref="K3">INDEX(K5:K7,$A$4)</f>
+        <v>IE-LH</v>
+      </c>
+      <c r="L3" s="3" t="str" cm="1">
+        <f t="array" ref="L3">INDEX(L5:L7,$A$4)</f>
+        <v>IE-MH</v>
+      </c>
+      <c r="M3" s="3" t="str" cm="1">
+        <f t="array" ref="M3">INDEX(M5:M7,$A$4)</f>
+        <v>IE-OY</v>
+      </c>
+      <c r="N3" s="3" t="str" cm="1">
+        <f t="array" ref="N3">INDEX(N5:N7,$A$4)</f>
+        <v>IE-WH</v>
+      </c>
+      <c r="O3" s="3" t="str" cm="1">
+        <f t="array" ref="O3">INDEX(O5:O7,$A$4)</f>
+        <v>IE-WX</v>
+      </c>
+      <c r="P3" s="3" t="str" cm="1">
+        <f t="array" ref="P3">INDEX(P5:P7,$A$4)</f>
+        <v>IE-WW</v>
+      </c>
+      <c r="Q3" s="3" t="str" cm="1">
+        <f t="array" ref="Q3">INDEX(Q5:Q7,$A$4)</f>
+        <v>IE-CE</v>
+      </c>
+      <c r="R3" s="3" t="str" cm="1">
+        <f t="array" ref="R3">INDEX(R5:R7,$A$4)</f>
+        <v>IE-CO</v>
+      </c>
+      <c r="S3" s="3" t="str" cm="1">
+        <f t="array" ref="S3">INDEX(S5:S7,$A$4)</f>
+        <v>IE-KY</v>
+      </c>
+      <c r="T3" s="3" t="str" cm="1">
+        <f t="array" ref="T3">INDEX(T5:T7,$A$4)</f>
+        <v>IE-LK</v>
+      </c>
+      <c r="U3" s="3" t="str" cm="1">
+        <f t="array" ref="U3">INDEX(U5:U7,$A$4)</f>
+        <v>IE-TA</v>
+      </c>
+      <c r="V3" s="3" t="str" cm="1">
+        <f t="array" ref="V3">INDEX(V5:V7,$A$4)</f>
+        <v>IE-WD</v>
+      </c>
+      <c r="W3" s="3" t="str" cm="1">
+        <f t="array" ref="W3">INDEX(W5:W7,$A$4)</f>
+        <v>IE-G</v>
+      </c>
+      <c r="X3" s="3" t="str" cm="1">
+        <f t="array" ref="X3">INDEX(X5:X7,$A$4)</f>
+        <v>IE-LM</v>
+      </c>
+      <c r="Y3" s="3" t="str" cm="1">
+        <f t="array" ref="Y3">INDEX(Y5:Y7,$A$4)</f>
+        <v>IE-MO</v>
+      </c>
+      <c r="Z3" s="3" t="str" cm="1">
+        <f t="array" ref="Z3">INDEX(Z5:Z7,$A$4)</f>
+        <v>IE-RN</v>
+      </c>
+      <c r="AA3" s="3" t="str" cm="1">
+        <f t="array" ref="AA3">INDEX(AA5:AA7,$A$4)</f>
+        <v>IE-SO</v>
+      </c>
+      <c r="AB3" s="3" t="str" cm="1">
+        <f t="array" ref="AB3">INDEX(AB5:AB7,$A$4)</f>
+        <v>IE-CN</v>
+      </c>
+      <c r="AC3" s="3" t="str" cm="1">
+        <f t="array" ref="AC3">INDEX(AC5:AC7,$A$4)</f>
+        <v>IE-DL</v>
+      </c>
+      <c r="AD3" s="3" t="str" cm="1">
+        <f t="array" ref="AD3">INDEX(AD5:AD7,$A$4)</f>
+        <v>IE-MN</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="15">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="3" t="str">
+        <f>A11</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="F5" s="3" t="str">
+        <f>A16</f>
+        <v>IE-D</v>
+      </c>
+      <c r="G5" s="3" t="str">
+        <f>A19</f>
+        <v>IE-KE</v>
+      </c>
+      <c r="H5" s="3" t="str">
+        <f>A20</f>
+        <v>IE-KK</v>
+      </c>
+      <c r="I5" s="3" t="str">
+        <f>A21</f>
+        <v>IE-LS</v>
+      </c>
+      <c r="J5" s="3" t="str">
+        <f>A24</f>
+        <v>IE-LD</v>
+      </c>
+      <c r="K5" s="3" t="str">
+        <f>A25</f>
+        <v>IE-LH</v>
+      </c>
+      <c r="L5" s="3" t="str">
+        <f>A27</f>
+        <v>IE-MH</v>
+      </c>
+      <c r="M5" s="3" t="str">
+        <f>A29</f>
+        <v>IE-OY</v>
+      </c>
+      <c r="N5" s="3" t="str">
+        <f>A34</f>
+        <v>IE-WH</v>
+      </c>
+      <c r="O5" s="3" t="str">
+        <f>A35</f>
+        <v>IE-WX</v>
+      </c>
+      <c r="P5" s="3" t="str">
+        <f>A36</f>
+        <v>IE-WW</v>
+      </c>
+      <c r="Q5" s="3" t="str">
+        <f>A13</f>
+        <v>IE-CE</v>
+      </c>
+      <c r="R5" s="3" t="str">
+        <f>A14</f>
+        <v>IE-CO</v>
+      </c>
+      <c r="S5" s="3" t="str">
+        <f>A18</f>
+        <v>IE-KY</v>
+      </c>
+      <c r="T5" s="3" t="str">
+        <f>A23</f>
+        <v>IE-LK</v>
+      </c>
+      <c r="U5" s="3" t="str">
+        <f>A32</f>
+        <v>IE-TA</v>
+      </c>
+      <c r="V5" s="3" t="str">
+        <f>A33</f>
+        <v>IE-WD</v>
+      </c>
+      <c r="W5" s="3" t="str">
+        <f>A17</f>
+        <v>IE-G</v>
+      </c>
+      <c r="X5" s="3" t="str">
+        <f>A22</f>
+        <v>IE-LM</v>
+      </c>
+      <c r="Y5" s="3" t="str">
+        <f>A26</f>
+        <v>IE-MO</v>
+      </c>
+      <c r="Z5" s="3" t="str">
+        <f>A30</f>
+        <v>IE-RN</v>
+      </c>
+      <c r="AA5" s="3" t="str">
+        <f>A31</f>
+        <v>IE-SO</v>
+      </c>
+      <c r="AB5" s="3" t="str">
+        <f>A12</f>
+        <v>IE-CN</v>
+      </c>
+      <c r="AC5" s="3" t="str">
+        <f>A15</f>
+        <v>IE-DL</v>
+      </c>
+      <c r="AD5" s="3" t="str">
+        <f>A28</f>
+        <v>IE-MN</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="15">
+      <c r="A6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="3" t="str">
+        <f>C5</f>
+        <v>IE</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>"*"&amp;D5</f>
+        <v>*National</v>
+      </c>
+      <c r="E6" s="3" t="str">
+        <f>"*"&amp;E5</f>
+        <v>*IE-CW</v>
+      </c>
+      <c r="F6" s="3" t="str">
+        <f t="shared" ref="F6:AD6" si="0">"*"&amp;F5</f>
+        <v>*IE-D</v>
+      </c>
+      <c r="G6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-KE</v>
+      </c>
+      <c r="H6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-KK</v>
+      </c>
+      <c r="I6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LS</v>
+      </c>
+      <c r="J6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LD</v>
+      </c>
+      <c r="K6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LH</v>
+      </c>
+      <c r="L6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-MH</v>
+      </c>
+      <c r="M6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-OY</v>
+      </c>
+      <c r="N6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-WH</v>
+      </c>
+      <c r="O6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-WX</v>
+      </c>
+      <c r="P6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-WW</v>
+      </c>
+      <c r="Q6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-CE</v>
+      </c>
+      <c r="R6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-CO</v>
+      </c>
+      <c r="S6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-KY</v>
+      </c>
+      <c r="T6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LK</v>
+      </c>
+      <c r="U6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-TA</v>
+      </c>
+      <c r="V6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-WD</v>
+      </c>
+      <c r="W6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-G</v>
+      </c>
+      <c r="X6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LM</v>
+      </c>
+      <c r="Y6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-MO</v>
+      </c>
+      <c r="Z6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-RN</v>
+      </c>
+      <c r="AA6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-SO</v>
+      </c>
+      <c r="AB6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-CN</v>
+      </c>
+      <c r="AC6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-DL</v>
+      </c>
+      <c r="AD6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-MN</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="15">
+      <c r="A7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3" t="str">
+        <f>"*"&amp;C5</f>
+        <v>*IE</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>D5</f>
+        <v>National</v>
+      </c>
+      <c r="E7" s="3" t="str">
+        <f t="shared" ref="E7:AD7" si="1">E5</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="F7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-D</v>
+      </c>
+      <c r="G7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-KE</v>
+      </c>
+      <c r="H7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-KK</v>
+      </c>
+      <c r="I7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LS</v>
+      </c>
+      <c r="J7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LD</v>
+      </c>
+      <c r="K7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LH</v>
+      </c>
+      <c r="L7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-MH</v>
+      </c>
+      <c r="M7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-OY</v>
+      </c>
+      <c r="N7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-WH</v>
+      </c>
+      <c r="O7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-WX</v>
+      </c>
+      <c r="P7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-WW</v>
+      </c>
+      <c r="Q7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-CE</v>
+      </c>
+      <c r="R7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-CO</v>
+      </c>
+      <c r="S7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-KY</v>
+      </c>
+      <c r="T7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LK</v>
+      </c>
+      <c r="U7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-TA</v>
+      </c>
+      <c r="V7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-WD</v>
+      </c>
+      <c r="W7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-G</v>
+      </c>
+      <c r="X7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LM</v>
+      </c>
+      <c r="Y7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-MO</v>
+      </c>
+      <c r="Z7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-RN</v>
+      </c>
+      <c r="AA7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-SO</v>
+      </c>
+      <c r="AB7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-CN</v>
+      </c>
+      <c r="AC7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-DL</v>
+      </c>
+      <c r="AD7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-MN</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="15.75" thickBot="1">
+      <c r="A10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30">
+      <c r="A12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30">
+      <c r="A13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
+      <c r="A14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30">
+      <c r="A15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30">
+      <c r="A16" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15">
+      <c r="A37" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId4" name="Drop Down 1">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="F14:T14"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" customWidth="1"/>
-    <col min="10" max="10" width="11.08984375" customWidth="1"/>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="10.75" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23">
       <c r="B1">
         <v>2015</v>
       </c>
@@ -587,7 +1777,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -616,29 +1806,30 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23">
       <c r="B4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23">
+      <c r="C5" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="C6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23">
       <c r="M7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -647,7 +1838,7 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
         <v>2</v>
@@ -659,7 +1850,7 @@
         <v>5</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J8" t="s">
         <v>4</v>
@@ -704,21 +1895,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23">
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K9" t="s">
         <v>6</v>
       </c>
       <c r="L9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M9" t="s">
         <v>16</v>
@@ -761,18 +1952,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23">
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K10" t="s">
         <v>6</v>
       </c>
       <c r="L10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M10" t="s">
         <v>16</v>
@@ -806,18 +1997,18 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23">
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K11" t="s">
         <v>6</v>
       </c>
       <c r="L11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M11" t="s">
         <v>16</v>
@@ -851,18 +2042,18 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23">
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K12" t="s">
         <v>6</v>
       </c>
       <c r="L12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M12" t="s">
         <v>16</v>
@@ -896,18 +2087,18 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23">
       <c r="F13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K13" t="s">
         <v>6</v>
       </c>
       <c r="L13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M13" t="s">
         <v>16</v>
@@ -941,18 +2132,18 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23">
       <c r="F14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K14" t="s">
         <v>6</v>
       </c>
       <c r="L14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M14" t="s">
         <v>16</v>
@@ -986,21 +2177,21 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K15" t="s">
         <v>6</v>
       </c>
       <c r="L15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M15" t="s">
         <v>16</v>
@@ -1034,21 +2225,21 @@
         <v>-1.0000000000000009E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K16" t="s">
         <v>6</v>
       </c>
       <c r="L16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M16" t="s">
         <v>16</v>
@@ -1082,21 +2273,21 @@
         <v>-1.0000000000000009E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K17" t="s">
         <v>6</v>
       </c>
       <c r="L17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M17" t="s">
         <v>16</v>
@@ -1130,21 +2321,21 @@
         <v>-1.0000000000000009E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K18" t="s">
         <v>6</v>
       </c>
       <c r="L18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M18" t="s">
         <v>16</v>
@@ -1178,21 +2369,21 @@
         <v>-1.0000000000000009E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K19" t="s">
         <v>6</v>
       </c>
       <c r="L19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M19" t="s">
         <v>16</v>
@@ -1226,21 +2417,21 @@
         <v>-1.0000000000000009E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K20" t="s">
         <v>6</v>
       </c>
       <c r="L20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M20" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Simplify RES and Bio penetration constraints and get rid of VEDA notifications
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_RES99.xlsx
+++ b/SuppXLS/Scen_ELC_RES99.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A015F1AD-C5D2-419D-B4DC-F023D7B76D72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456C3A60-595B-4CF8-BB99-E088475CB908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,14 +72,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="82">
   <si>
     <t>UC_N</t>
   </si>
   <si>
-    <t>Pset_CI</t>
-  </si>
-  <si>
     <t>Pset_PN</t>
   </si>
   <si>
@@ -89,15 +86,9 @@
     <t>Cset_CN</t>
   </si>
   <si>
-    <t>Pset_CO</t>
-  </si>
-  <si>
     <t>UC_FLO</t>
   </si>
   <si>
-    <t>Attribute</t>
-  </si>
-  <si>
     <t>LimType</t>
   </si>
   <si>
@@ -113,88 +104,19 @@
     <t>UC_RHSRTS</t>
   </si>
   <si>
-    <t>UC_RES</t>
-  </si>
-  <si>
-    <t>RES Penetration</t>
-  </si>
-  <si>
     <t>UC_RHSRTS~0</t>
   </si>
   <si>
-    <t>UP</t>
-  </si>
-  <si>
-    <t>Top_Check</t>
-  </si>
-  <si>
     <t>RNW Level</t>
   </si>
   <si>
     <t>~UC_T</t>
   </si>
   <si>
-    <t>RNW Check (Renewable = 1)</t>
-  </si>
-  <si>
     <t>Pset_PD</t>
   </si>
   <si>
-    <t>Cset_SET</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>ELCC,ELCD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P*GAS*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P*COA*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P*OIL*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P*HYD*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P*WIN*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P*SOL*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P*BIO*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P*OCE*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P*GEO*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P*PEA*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P*DIS*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P*HFO*</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -394,6 +316,27 @@
       </rPr>
       <t>https://en.wikipedia.org/wiki/ISO_3166-2:IE</t>
     </r>
+  </si>
+  <si>
+    <t>P*RNW*</t>
+  </si>
+  <si>
+    <t>CHP,ELE</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>UC_COMPRD</t>
+  </si>
+  <si>
+    <t>LO</t>
+  </si>
+  <si>
+    <t>Minimum RES Penetration</t>
+  </si>
+  <si>
+    <t>UC_MinRES</t>
   </si>
 </sst>
 </file>
@@ -1104,13 +1047,13 @@
     </row>
     <row r="5" spans="1:30" ht="15">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3" t="str">
         <f>A11</f>
@@ -1219,7 +1162,7 @@
     </row>
     <row r="6" spans="1:30" ht="15">
       <c r="A6" s="2" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>C5</f>
@@ -1336,7 +1279,7 @@
     </row>
     <row r="7" spans="1:30" ht="15">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="str">
         <f>"*"&amp;C5</f>
@@ -1453,223 +1396,223 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1">
       <c r="A10" s="5" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:30">
       <c r="A11" s="6" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="7" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="7" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="7" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="7" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="7" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="7" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="7" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="7" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="7" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="7" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="7" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="7" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="7" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="7" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="7" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="7" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="7" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="7" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="7" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="7" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="7" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="7" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="7" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="7" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="7" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15">
       <c r="A37" s="8" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1711,10 +1654,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="G10" sqref="G10:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1726,7 +1669,7 @@
     <col min="10" max="10" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:14">
       <c r="B1">
         <v>2015</v>
       </c>
@@ -1752,9 +1695,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1781,663 +1724,175 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23">
-      <c r="C5" t="str">
+    <row r="5" spans="1:14">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="str">
         <f>_xlfn.TEXTJOIN(" ",TRUE,"~UC_Sets: R_E:",_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,"")))</f>
         <v>~UC_Sets: R_E: IE,National</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
-      <c r="C6" t="s">
+    <row r="7" spans="1:14">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="I8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="C9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:23">
-      <c r="M7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="M9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="C10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2020</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <f>-$C$2</f>
+        <v>-0.1</v>
+      </c>
+      <c r="L10" s="2">
         <v>0</v>
       </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" t="s">
-        <v>8</v>
-      </c>
-      <c r="N8">
-        <v>2020</v>
-      </c>
-      <c r="O8">
+      <c r="M10" s="2">
+        <v>15</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="G11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="2">
         <v>2025</v>
       </c>
-      <c r="P8">
+      <c r="K11" s="2">
+        <f>-$D$2</f>
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="G12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="2">
         <v>2030</v>
       </c>
-      <c r="Q8">
+      <c r="K12" s="2">
+        <f>-$E$2</f>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="G13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="2">
         <v>2035</v>
       </c>
-      <c r="R8">
+      <c r="K13" s="2">
+        <f>-$F$2</f>
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="G14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="2">
         <v>2040</v>
       </c>
-      <c r="S8">
+      <c r="K14" s="2">
+        <f>-$G$2</f>
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="G15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="2">
         <v>2045</v>
       </c>
-      <c r="T8">
+      <c r="K15" s="2">
+        <f>-$H$2</f>
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="G16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="2">
         <v>2050</v>
       </c>
-      <c r="U8" t="s">
-        <v>12</v>
-      </c>
-      <c r="V8" t="s">
-        <v>10</v>
-      </c>
-      <c r="W8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23">
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" t="s">
-        <v>16</v>
-      </c>
-      <c r="N9">
-        <f>IF($A9=1,C$2-1,C$2)</f>
-        <v>0.1</v>
-      </c>
-      <c r="O9">
-        <f t="shared" ref="O9:T9" si="0">IF($A9=1,D$2-1,D$2)</f>
-        <v>0.3</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9" t="s">
-        <v>14</v>
-      </c>
-      <c r="W9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23">
-      <c r="F10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" t="s">
-        <v>16</v>
-      </c>
-      <c r="N10">
-        <f t="shared" ref="N10:N18" si="1">IF($A10=1,C$2-1,C$2)</f>
-        <v>0.1</v>
-      </c>
-      <c r="O10">
-        <f t="shared" ref="O10:O18" si="2">IF($A10=1,D$2-1,D$2)</f>
-        <v>0.3</v>
-      </c>
-      <c r="P10">
-        <f t="shared" ref="P10:P18" si="3">IF($A10=1,E$2-1,E$2)</f>
-        <v>0.5</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" ref="Q10:Q18" si="4">IF($A10=1,F$2-1,F$2)</f>
-        <v>0.6</v>
-      </c>
-      <c r="R10">
-        <f t="shared" ref="R10:R18" si="5">IF($A10=1,G$2-1,G$2)</f>
-        <v>0.7</v>
-      </c>
-      <c r="S10">
-        <f t="shared" ref="S10:S18" si="6">IF($A10=1,H$2-1,H$2)</f>
-        <v>0.8</v>
-      </c>
-      <c r="T10">
-        <f t="shared" ref="T10:T18" si="7">IF($A10=1,I$2-1,I$2)</f>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23">
-      <c r="F11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" t="s">
-        <v>6</v>
-      </c>
-      <c r="L11" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11">
-        <f t="shared" ref="N11" si="8">IF($A11=1,C$2-1,C$2)</f>
-        <v>0.1</v>
-      </c>
-      <c r="O11">
-        <f t="shared" ref="O11" si="9">IF($A11=1,D$2-1,D$2)</f>
-        <v>0.3</v>
-      </c>
-      <c r="P11">
-        <f t="shared" ref="P11" si="10">IF($A11=1,E$2-1,E$2)</f>
-        <v>0.5</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" ref="Q11" si="11">IF($A11=1,F$2-1,F$2)</f>
-        <v>0.6</v>
-      </c>
-      <c r="R11">
-        <f t="shared" ref="R11" si="12">IF($A11=1,G$2-1,G$2)</f>
-        <v>0.7</v>
-      </c>
-      <c r="S11">
-        <f t="shared" ref="S11" si="13">IF($A11=1,H$2-1,H$2)</f>
-        <v>0.8</v>
-      </c>
-      <c r="T11">
-        <f t="shared" ref="T11" si="14">IF($A11=1,I$2-1,I$2)</f>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23">
-      <c r="F12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L12" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="2"/>
-        <v>0.3</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="4"/>
-        <v>0.6</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="5"/>
-        <v>0.7</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="6"/>
-        <v>0.8</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="7"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23">
-      <c r="F13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" t="s">
-        <v>16</v>
-      </c>
-      <c r="N13">
-        <f t="shared" ref="N13" si="15">IF($A13=1,C$2-1,C$2)</f>
-        <v>0.1</v>
-      </c>
-      <c r="O13">
-        <f t="shared" ref="O13" si="16">IF($A13=1,D$2-1,D$2)</f>
-        <v>0.3</v>
-      </c>
-      <c r="P13">
-        <f t="shared" ref="P13" si="17">IF($A13=1,E$2-1,E$2)</f>
-        <v>0.5</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" ref="Q13" si="18">IF($A13=1,F$2-1,F$2)</f>
-        <v>0.6</v>
-      </c>
-      <c r="R13">
-        <f t="shared" ref="R13" si="19">IF($A13=1,G$2-1,G$2)</f>
-        <v>0.7</v>
-      </c>
-      <c r="S13">
-        <f t="shared" ref="S13" si="20">IF($A13=1,H$2-1,H$2)</f>
-        <v>0.8</v>
-      </c>
-      <c r="T13">
-        <f t="shared" ref="T13" si="21">IF($A13=1,I$2-1,I$2)</f>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23">
-      <c r="F14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" t="s">
-        <v>6</v>
-      </c>
-      <c r="L14" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" t="s">
-        <v>16</v>
-      </c>
-      <c r="N14">
-        <f t="shared" ref="N14" si="22">IF($A14=1,C$2-1,C$2)</f>
-        <v>0.1</v>
-      </c>
-      <c r="O14">
-        <f t="shared" ref="O14" si="23">IF($A14=1,D$2-1,D$2)</f>
-        <v>0.3</v>
-      </c>
-      <c r="P14">
-        <f t="shared" ref="P14" si="24">IF($A14=1,E$2-1,E$2)</f>
-        <v>0.5</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" ref="Q14" si="25">IF($A14=1,F$2-1,F$2)</f>
-        <v>0.6</v>
-      </c>
-      <c r="R14">
-        <f t="shared" ref="R14" si="26">IF($A14=1,G$2-1,G$2)</f>
-        <v>0.7</v>
-      </c>
-      <c r="S14">
-        <f t="shared" ref="S14" si="27">IF($A14=1,H$2-1,H$2)</f>
-        <v>0.8</v>
-      </c>
-      <c r="T14">
-        <f t="shared" ref="T14" si="28">IF($A14=1,I$2-1,I$2)</f>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J15" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" t="s">
-        <v>16</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="1"/>
-        <v>-0.9</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="2"/>
-        <v>-0.7</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="3"/>
-        <v>-0.5</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="4"/>
-        <v>-0.4</v>
-      </c>
-      <c r="R15">
-        <f t="shared" si="5"/>
-        <v>-0.30000000000000004</v>
-      </c>
-      <c r="S15">
-        <f t="shared" si="6"/>
-        <v>-0.19999999999999996</v>
-      </c>
-      <c r="T15">
-        <f t="shared" si="7"/>
-        <v>-1.0000000000000009E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J16" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" t="s">
-        <v>6</v>
-      </c>
-      <c r="L16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="1"/>
-        <v>-0.9</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="2"/>
-        <v>-0.7</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="3"/>
-        <v>-0.5</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="4"/>
-        <v>-0.4</v>
-      </c>
-      <c r="R16">
-        <f t="shared" si="5"/>
-        <v>-0.30000000000000004</v>
-      </c>
-      <c r="S16">
-        <f t="shared" si="6"/>
-        <v>-0.19999999999999996</v>
-      </c>
-      <c r="T16">
-        <f t="shared" si="7"/>
-        <v>-1.0000000000000009E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J17" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L17" t="s">
-        <v>23</v>
-      </c>
-      <c r="M17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="1"/>
-        <v>-0.9</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="2"/>
-        <v>-0.7</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="3"/>
-        <v>-0.5</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="4"/>
-        <v>-0.4</v>
-      </c>
-      <c r="R17">
-        <f t="shared" si="5"/>
-        <v>-0.30000000000000004</v>
-      </c>
-      <c r="S17">
-        <f t="shared" si="6"/>
-        <v>-0.19999999999999996</v>
-      </c>
-      <c r="T17">
-        <f t="shared" si="7"/>
-        <v>-1.0000000000000009E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J18" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" t="s">
-        <v>6</v>
-      </c>
-      <c r="L18" t="s">
-        <v>23</v>
-      </c>
-      <c r="M18" t="s">
-        <v>16</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="1"/>
-        <v>-0.9</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="2"/>
-        <v>-0.7</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="3"/>
-        <v>-0.5</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="4"/>
-        <v>-0.4</v>
-      </c>
-      <c r="R18">
-        <f t="shared" si="5"/>
-        <v>-0.30000000000000004</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="6"/>
-        <v>-0.19999999999999996</v>
-      </c>
-      <c r="T18">
-        <f t="shared" si="7"/>
-        <v>-1.0000000000000009E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J19" t="s">
-        <v>24</v>
-      </c>
-      <c r="K19" t="s">
-        <v>6</v>
-      </c>
-      <c r="L19" t="s">
-        <v>23</v>
-      </c>
-      <c r="M19" t="s">
-        <v>16</v>
-      </c>
-      <c r="N19">
-        <f t="shared" ref="N19:T20" si="29">IF($A19=1,C$2-1,C$2)</f>
-        <v>-0.9</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="29"/>
-        <v>-0.7</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="29"/>
-        <v>-0.5</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="29"/>
-        <v>-0.4</v>
-      </c>
-      <c r="R19">
-        <f t="shared" si="29"/>
-        <v>-0.30000000000000004</v>
-      </c>
-      <c r="S19">
-        <f t="shared" si="29"/>
-        <v>-0.19999999999999996</v>
-      </c>
-      <c r="T19">
-        <f t="shared" si="29"/>
-        <v>-1.0000000000000009E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J20" t="s">
-        <v>24</v>
-      </c>
-      <c r="K20" t="s">
-        <v>6</v>
-      </c>
-      <c r="L20" t="s">
-        <v>23</v>
-      </c>
-      <c r="M20" t="s">
-        <v>16</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="29"/>
-        <v>-0.9</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="29"/>
-        <v>-0.7</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="29"/>
-        <v>-0.5</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="29"/>
-        <v>-0.4</v>
-      </c>
-      <c r="R20">
-        <f t="shared" si="29"/>
-        <v>-0.30000000000000004</v>
-      </c>
-      <c r="S20">
-        <f t="shared" si="29"/>
-        <v>-0.19999999999999996</v>
-      </c>
-      <c r="T20">
-        <f t="shared" si="29"/>
-        <v>-1.0000000000000009E-2</v>
+      <c r="K16" s="2">
+        <f>-$I$2</f>
+        <v>-0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>